<commit_message>
deseq-analysis, reporter hill fit scatters with errors
</commit_message>
<xml_diff>
--- a/data/malathion-reporter-plate-reader/plate_layouts.xlsx
+++ b/data/malathion-reporter-plate-reader/plate_layouts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aqib/Desktop/BCCL/koopman-sensor-placement/NC_submission/transcriptome-dynamics-dmd-observability/data/malathion-reporter-plate-reader/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC8731C-65F3-F949-888C-9B71AFC13EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD57758-7BEB-864E-869E-F4D4F8EF6097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43060" yWindow="1740" windowWidth="28040" windowHeight="17440" xr2:uid="{86E41D9F-BC50-BD4C-BFC8-A140258F459E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{86E41D9F-BC50-BD4C-BFC8-A140258F459E}"/>
   </bookViews>
   <sheets>
     <sheet name="h1_specificity_09.09.22" sheetId="1" r:id="rId1"/>
@@ -199,6 +199,222 @@
     <t>4736_perm_2</t>
   </si>
   <si>
+    <t>4150_control_0</t>
+  </si>
+  <si>
+    <t>4150_control_1</t>
+  </si>
+  <si>
+    <t>4150_control_2</t>
+  </si>
+  <si>
+    <t>4150_zeta_0</t>
+  </si>
+  <si>
+    <t>4150_zeta_1</t>
+  </si>
+  <si>
+    <t>4150_zeta_2</t>
+  </si>
+  <si>
+    <t>4150_perm_0</t>
+  </si>
+  <si>
+    <t>4150_perm_1</t>
+  </si>
+  <si>
+    <t>4150_perm_2</t>
+  </si>
+  <si>
+    <t>0376_control_0</t>
+  </si>
+  <si>
+    <t>0376_control_1</t>
+  </si>
+  <si>
+    <t>0376_control_2</t>
+  </si>
+  <si>
+    <t>0376_zeta_0</t>
+  </si>
+  <si>
+    <t>0376_zeta_1</t>
+  </si>
+  <si>
+    <t>0376_zeta_2</t>
+  </si>
+  <si>
+    <t>0376_perm_0</t>
+  </si>
+  <si>
+    <t>0376_perm_1</t>
+  </si>
+  <si>
+    <t>0376_perm_2</t>
+  </si>
+  <si>
+    <t>1815_control_0</t>
+  </si>
+  <si>
+    <t>1815_control_1</t>
+  </si>
+  <si>
+    <t>1815_control_2</t>
+  </si>
+  <si>
+    <t>1815_zeta_0</t>
+  </si>
+  <si>
+    <t>1815_zeta_1</t>
+  </si>
+  <si>
+    <t>1815_zeta_2</t>
+  </si>
+  <si>
+    <t>1815_perm_0</t>
+  </si>
+  <si>
+    <t>1815_perm_1</t>
+  </si>
+  <si>
+    <t>1815_perm_2</t>
+  </si>
+  <si>
+    <t>0953_control_0</t>
+  </si>
+  <si>
+    <t>0953_control_1</t>
+  </si>
+  <si>
+    <t>0953_control_2</t>
+  </si>
+  <si>
+    <t>0953_zeta_0</t>
+  </si>
+  <si>
+    <t>0953_zeta_1</t>
+  </si>
+  <si>
+    <t>0953_zeta_2</t>
+  </si>
+  <si>
+    <t>0953_perm_0</t>
+  </si>
+  <si>
+    <t>0953_perm_1</t>
+  </si>
+  <si>
+    <t>0953_perm_2</t>
+  </si>
+  <si>
+    <t>1358_control_0</t>
+  </si>
+  <si>
+    <t>1358_control_1</t>
+  </si>
+  <si>
+    <t>1358_control_2</t>
+  </si>
+  <si>
+    <t>1358_zeta_0</t>
+  </si>
+  <si>
+    <t>1358_zeta_1</t>
+  </si>
+  <si>
+    <t>1358_zeta_2</t>
+  </si>
+  <si>
+    <t>1358_perm_0</t>
+  </si>
+  <si>
+    <t>1358_perm_1</t>
+  </si>
+  <si>
+    <t>1358_perm_2</t>
+  </si>
+  <si>
+    <t>1302A_control_0</t>
+  </si>
+  <si>
+    <t>1302A_control_1</t>
+  </si>
+  <si>
+    <t>1302A_control_2</t>
+  </si>
+  <si>
+    <t>1302A_zeta_0</t>
+  </si>
+  <si>
+    <t>1302A_zeta_1</t>
+  </si>
+  <si>
+    <t>1302A_zeta_2</t>
+  </si>
+  <si>
+    <t>1302A_perm_0</t>
+  </si>
+  <si>
+    <t>1302A_perm_1</t>
+  </si>
+  <si>
+    <t>1302A_perm_2</t>
+  </si>
+  <si>
+    <t>4612_control_0</t>
+  </si>
+  <si>
+    <t>4612_control_1</t>
+  </si>
+  <si>
+    <t>4612_control_2</t>
+  </si>
+  <si>
+    <t>4612_zeta_0</t>
+  </si>
+  <si>
+    <t>4612_zeta_1</t>
+  </si>
+  <si>
+    <t>4612_zeta_2</t>
+  </si>
+  <si>
+    <t>4612_perm_0</t>
+  </si>
+  <si>
+    <t>4612_perm_1</t>
+  </si>
+  <si>
+    <t>4612_perm_2</t>
+  </si>
+  <si>
+    <t>1380_control_0</t>
+  </si>
+  <si>
+    <t>1380_control_1</t>
+  </si>
+  <si>
+    <t>1380_control_2</t>
+  </si>
+  <si>
+    <t>1380_zeta_0</t>
+  </si>
+  <si>
+    <t>1380_zeta_1</t>
+  </si>
+  <si>
+    <t>1380_zeta_2</t>
+  </si>
+  <si>
+    <t>1380_perm_0</t>
+  </si>
+  <si>
+    <t>1380_perm_1</t>
+  </si>
+  <si>
+    <t>1380_perm_2</t>
+  </si>
+  <si>
     <t>3761_control_0</t>
   </si>
   <si>
@@ -224,222 +440,6 @@
   </si>
   <si>
     <t>3761_perm_2</t>
-  </si>
-  <si>
-    <t>4150_control_0</t>
-  </si>
-  <si>
-    <t>4150_control_1</t>
-  </si>
-  <si>
-    <t>4150_control_2</t>
-  </si>
-  <si>
-    <t>4150_zeta_0</t>
-  </si>
-  <si>
-    <t>4150_zeta_1</t>
-  </si>
-  <si>
-    <t>4150_zeta_2</t>
-  </si>
-  <si>
-    <t>4150_perm_0</t>
-  </si>
-  <si>
-    <t>4150_perm_1</t>
-  </si>
-  <si>
-    <t>4150_perm_2</t>
-  </si>
-  <si>
-    <t>0376_control_0</t>
-  </si>
-  <si>
-    <t>0376_control_1</t>
-  </si>
-  <si>
-    <t>0376_control_2</t>
-  </si>
-  <si>
-    <t>0376_zeta_0</t>
-  </si>
-  <si>
-    <t>0376_zeta_1</t>
-  </si>
-  <si>
-    <t>0376_zeta_2</t>
-  </si>
-  <si>
-    <t>0376_perm_0</t>
-  </si>
-  <si>
-    <t>0376_perm_1</t>
-  </si>
-  <si>
-    <t>0376_perm_2</t>
-  </si>
-  <si>
-    <t>1815_control_0</t>
-  </si>
-  <si>
-    <t>1815_control_1</t>
-  </si>
-  <si>
-    <t>1815_control_2</t>
-  </si>
-  <si>
-    <t>1815_zeta_0</t>
-  </si>
-  <si>
-    <t>1815_zeta_1</t>
-  </si>
-  <si>
-    <t>1815_zeta_2</t>
-  </si>
-  <si>
-    <t>1815_perm_0</t>
-  </si>
-  <si>
-    <t>1815_perm_1</t>
-  </si>
-  <si>
-    <t>1815_perm_2</t>
-  </si>
-  <si>
-    <t>0953_control_0</t>
-  </si>
-  <si>
-    <t>0953_control_1</t>
-  </si>
-  <si>
-    <t>0953_control_2</t>
-  </si>
-  <si>
-    <t>0953_zeta_0</t>
-  </si>
-  <si>
-    <t>0953_zeta_1</t>
-  </si>
-  <si>
-    <t>0953_zeta_2</t>
-  </si>
-  <si>
-    <t>0953_perm_0</t>
-  </si>
-  <si>
-    <t>0953_perm_1</t>
-  </si>
-  <si>
-    <t>0953_perm_2</t>
-  </si>
-  <si>
-    <t>1358_control_0</t>
-  </si>
-  <si>
-    <t>1358_control_1</t>
-  </si>
-  <si>
-    <t>1358_control_2</t>
-  </si>
-  <si>
-    <t>1358_zeta_0</t>
-  </si>
-  <si>
-    <t>1358_zeta_1</t>
-  </si>
-  <si>
-    <t>1358_zeta_2</t>
-  </si>
-  <si>
-    <t>1358_perm_0</t>
-  </si>
-  <si>
-    <t>1358_perm_1</t>
-  </si>
-  <si>
-    <t>1358_perm_2</t>
-  </si>
-  <si>
-    <t>1302A_control_0</t>
-  </si>
-  <si>
-    <t>1302A_control_1</t>
-  </si>
-  <si>
-    <t>1302A_control_2</t>
-  </si>
-  <si>
-    <t>1302A_zeta_0</t>
-  </si>
-  <si>
-    <t>1302A_zeta_1</t>
-  </si>
-  <si>
-    <t>1302A_zeta_2</t>
-  </si>
-  <si>
-    <t>1302A_perm_0</t>
-  </si>
-  <si>
-    <t>1302A_perm_1</t>
-  </si>
-  <si>
-    <t>1302A_perm_2</t>
-  </si>
-  <si>
-    <t>4612_control_0</t>
-  </si>
-  <si>
-    <t>4612_control_1</t>
-  </si>
-  <si>
-    <t>4612_control_2</t>
-  </si>
-  <si>
-    <t>4612_zeta_0</t>
-  </si>
-  <si>
-    <t>4612_zeta_1</t>
-  </si>
-  <si>
-    <t>4612_zeta_2</t>
-  </si>
-  <si>
-    <t>4612_perm_0</t>
-  </si>
-  <si>
-    <t>4612_perm_1</t>
-  </si>
-  <si>
-    <t>4612_perm_2</t>
-  </si>
-  <si>
-    <t>1380_control_0</t>
-  </si>
-  <si>
-    <t>1380_control_1</t>
-  </si>
-  <si>
-    <t>1380_control_2</t>
-  </si>
-  <si>
-    <t>1380_zeta_0</t>
-  </si>
-  <si>
-    <t>1380_zeta_1</t>
-  </si>
-  <si>
-    <t>1380_zeta_2</t>
-  </si>
-  <si>
-    <t>1380_perm_0</t>
-  </si>
-  <si>
-    <t>1380_perm_1</t>
-  </si>
-  <si>
-    <t>1380_perm_2</t>
   </si>
 </sst>
 </file>
@@ -799,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C4EC1B-2C39-9543-AD5A-A443B66DD218}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -957,89 +957,89 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="G6" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="H6" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="I6" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F7" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="G7" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="H7" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="I7" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="F8" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="G8" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="H8" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="I8" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1052,8 +1052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE6610B7-8CB1-BB4F-B087-1EB669BFFD36}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScale="183" zoomScaleNormal="183" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1065,205 +1065,205 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>126</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>127</v>
       </c>
       <c r="C1" t="s">
-        <v>74</v>
+        <v>128</v>
       </c>
       <c r="D1" t="s">
-        <v>75</v>
+        <v>129</v>
       </c>
       <c r="E1" t="s">
-        <v>76</v>
+        <v>130</v>
       </c>
       <c r="F1" t="s">
-        <v>77</v>
+        <v>131</v>
       </c>
       <c r="G1" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="H1" t="s">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="I1" t="s">
-        <v>80</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="F2" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="H2" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="I2" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="E3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="F3" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="H3" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="I3" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="D4" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="E4" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="F4" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="G4" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="H4" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="I4" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="D5" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="E5" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="F5" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="G5" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="H5" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="I5" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="D6" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="E6" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="F6" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="G6" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="H6" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="I6" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C7" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D7" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="E7" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="F7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="G7" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="H7" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="I7" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correlation of mal with fru and lac
</commit_message>
<xml_diff>
--- a/data/malathion-reporter-plate-reader/plate_layouts.xlsx
+++ b/data/malathion-reporter-plate-reader/plate_layouts.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aqib/Desktop/BCCL/koopman-sensor-placement/NC_submission/transcriptome-dynamics-dmd-observability/data/malathion-reporter-plate-reader/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD57758-7BEB-864E-869E-F4D4F8EF6097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEFD971-40DA-464A-A40B-40606F764358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{86E41D9F-BC50-BD4C-BFC8-A140258F459E}"/>
   </bookViews>
   <sheets>
-    <sheet name="h1_specificity_09.09.22" sheetId="1" r:id="rId1"/>
-    <sheet name="neo2_specificity_09.09.22" sheetId="2" r:id="rId2"/>
+    <sheet name="h1_specificity_09.09.22" sheetId="4" r:id="rId1"/>
+    <sheet name="neo2_specificity_09.09.22" sheetId="3" r:id="rId2"/>
+    <sheet name="h1_specificity_09.13.22" sheetId="1" r:id="rId3"/>
+    <sheet name="neo2_specificity_09.13.22" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="225">
   <si>
     <t>6124_control_0</t>
   </si>
@@ -440,6 +442,276 @@
   </si>
   <si>
     <t>3761_perm_2</t>
+  </si>
+  <si>
+    <t>3761_fructose_0</t>
+  </si>
+  <si>
+    <t>3761_fructose_1</t>
+  </si>
+  <si>
+    <t>3761_fructose_2</t>
+  </si>
+  <si>
+    <t>0376_fructose_0</t>
+  </si>
+  <si>
+    <t>0376_fructose_1</t>
+  </si>
+  <si>
+    <t>0376_fructose_2</t>
+  </si>
+  <si>
+    <t>0953_fructose_0</t>
+  </si>
+  <si>
+    <t>0953_fructose_1</t>
+  </si>
+  <si>
+    <t>0953_fructose_2</t>
+  </si>
+  <si>
+    <t>4612_fructose_0</t>
+  </si>
+  <si>
+    <t>4612_fructose_1</t>
+  </si>
+  <si>
+    <t>4612_fructose_2</t>
+  </si>
+  <si>
+    <t>1358_fructose_0</t>
+  </si>
+  <si>
+    <t>1358_fructose_1</t>
+  </si>
+  <si>
+    <t>1358_fructose_2</t>
+  </si>
+  <si>
+    <t>1302A_fructose_0</t>
+  </si>
+  <si>
+    <t>1302A_fructose_1</t>
+  </si>
+  <si>
+    <t>1302A_fructose_2</t>
+  </si>
+  <si>
+    <t>1380_fructose_0</t>
+  </si>
+  <si>
+    <t>1380_fructose_1</t>
+  </si>
+  <si>
+    <t>1380_fructose_2</t>
+  </si>
+  <si>
+    <t>3761_lactose_0</t>
+  </si>
+  <si>
+    <t>3761_lactose_1</t>
+  </si>
+  <si>
+    <t>3761_lactose_2</t>
+  </si>
+  <si>
+    <t>0376_lactose_0</t>
+  </si>
+  <si>
+    <t>0376_lactose_1</t>
+  </si>
+  <si>
+    <t>0376_lactose_2</t>
+  </si>
+  <si>
+    <t>0953_lactose_0</t>
+  </si>
+  <si>
+    <t>0953_lactose_1</t>
+  </si>
+  <si>
+    <t>0953_lactose_2</t>
+  </si>
+  <si>
+    <t>4612_lactose_0</t>
+  </si>
+  <si>
+    <t>4612_lactose_1</t>
+  </si>
+  <si>
+    <t>4612_lactose_2</t>
+  </si>
+  <si>
+    <t>1358_lactose_0</t>
+  </si>
+  <si>
+    <t>1358_lactose_1</t>
+  </si>
+  <si>
+    <t>1358_lactose_2</t>
+  </si>
+  <si>
+    <t>1302A_lactose_0</t>
+  </si>
+  <si>
+    <t>1302A_lactose_1</t>
+  </si>
+  <si>
+    <t>1302A_lactose_2</t>
+  </si>
+  <si>
+    <t>1380_lactose_0</t>
+  </si>
+  <si>
+    <t>1380_lactose_1</t>
+  </si>
+  <si>
+    <t>1380_lactose_2</t>
+  </si>
+  <si>
+    <t>6124_lactose_0</t>
+  </si>
+  <si>
+    <t>6124_lactose_1</t>
+  </si>
+  <si>
+    <t>6124_lactose_2</t>
+  </si>
+  <si>
+    <t>0841_lactose_0</t>
+  </si>
+  <si>
+    <t>0841_lactose_1</t>
+  </si>
+  <si>
+    <t>0841_lactose_2</t>
+  </si>
+  <si>
+    <t>1823_lactose_0</t>
+  </si>
+  <si>
+    <t>1823_lactose_1</t>
+  </si>
+  <si>
+    <t>1823_lactose_2</t>
+  </si>
+  <si>
+    <t>5502_lactose_0</t>
+  </si>
+  <si>
+    <t>5502_lactose_1</t>
+  </si>
+  <si>
+    <t>5502_lactose_2</t>
+  </si>
+  <si>
+    <t>1836_lactose_0</t>
+  </si>
+  <si>
+    <t>1836_lactose_1</t>
+  </si>
+  <si>
+    <t>1836_lactose_2</t>
+  </si>
+  <si>
+    <t>1815_lactose_0</t>
+  </si>
+  <si>
+    <t>1815_lactose_1</t>
+  </si>
+  <si>
+    <t>1815_lactose_2</t>
+  </si>
+  <si>
+    <t>4736_lactose_0</t>
+  </si>
+  <si>
+    <t>4736_lactose_1</t>
+  </si>
+  <si>
+    <t>4736_lactose_2</t>
+  </si>
+  <si>
+    <t>4150_lactose_0</t>
+  </si>
+  <si>
+    <t>4150_lactose_1</t>
+  </si>
+  <si>
+    <t>4150_lactose_2</t>
+  </si>
+  <si>
+    <t>6124_fructose_0</t>
+  </si>
+  <si>
+    <t>6124_fructose_1</t>
+  </si>
+  <si>
+    <t>6124_fructose_2</t>
+  </si>
+  <si>
+    <t>0841_fructose_0</t>
+  </si>
+  <si>
+    <t>0841_fructose_1</t>
+  </si>
+  <si>
+    <t>0841_fructose_2</t>
+  </si>
+  <si>
+    <t>1823_fructose_0</t>
+  </si>
+  <si>
+    <t>1823_fructose_1</t>
+  </si>
+  <si>
+    <t>1823_fructose_2</t>
+  </si>
+  <si>
+    <t>5502_fructose_0</t>
+  </si>
+  <si>
+    <t>5502_fructose_1</t>
+  </si>
+  <si>
+    <t>5502_fructose_2</t>
+  </si>
+  <si>
+    <t>1836_fructose_0</t>
+  </si>
+  <si>
+    <t>1836_fructose_1</t>
+  </si>
+  <si>
+    <t>1836_fructose_2</t>
+  </si>
+  <si>
+    <t>1815_fructose_0</t>
+  </si>
+  <si>
+    <t>1815_fructose_1</t>
+  </si>
+  <si>
+    <t>1815_fructose_2</t>
+  </si>
+  <si>
+    <t>4736_fructose_0</t>
+  </si>
+  <si>
+    <t>4736_fructose_1</t>
+  </si>
+  <si>
+    <t>4736_fructose_2</t>
+  </si>
+  <si>
+    <t>4150_fructose_0</t>
+  </si>
+  <si>
+    <t>4150_fructose_1</t>
+  </si>
+  <si>
+    <t>4150_fructose_2</t>
   </si>
 </sst>
 </file>
@@ -796,7 +1068,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C4EC1B-2C39-9543-AD5A-A443B66DD218}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5067E9B4-9539-074C-B754-EBBC23113DE7}">
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
@@ -1043,17 +1315,16 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE6610B7-8CB1-BB4F-B087-1EB669BFFD36}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{012CA423-6E37-EB41-BE63-F2F07D4939DA}">
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="183" zoomScaleNormal="183" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1269,4 +1540,480 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C4EC1B-2C39-9543-AD5A-A443B66DD218}">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E2" t="s">
+        <v>205</v>
+      </c>
+      <c r="F2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G2" t="s">
+        <v>180</v>
+      </c>
+      <c r="H2" t="s">
+        <v>181</v>
+      </c>
+      <c r="I2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E3" t="s">
+        <v>208</v>
+      </c>
+      <c r="F3" t="s">
+        <v>209</v>
+      </c>
+      <c r="G3" t="s">
+        <v>183</v>
+      </c>
+      <c r="H3" t="s">
+        <v>184</v>
+      </c>
+      <c r="I3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E4" t="s">
+        <v>211</v>
+      </c>
+      <c r="F4" t="s">
+        <v>212</v>
+      </c>
+      <c r="G4" t="s">
+        <v>186</v>
+      </c>
+      <c r="H4" t="s">
+        <v>187</v>
+      </c>
+      <c r="I4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F5" t="s">
+        <v>215</v>
+      </c>
+      <c r="G5" t="s">
+        <v>189</v>
+      </c>
+      <c r="H5" t="s">
+        <v>190</v>
+      </c>
+      <c r="I5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F6" t="s">
+        <v>218</v>
+      </c>
+      <c r="G6" t="s">
+        <v>192</v>
+      </c>
+      <c r="H6" t="s">
+        <v>193</v>
+      </c>
+      <c r="I6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" t="s">
+        <v>219</v>
+      </c>
+      <c r="E7" t="s">
+        <v>220</v>
+      </c>
+      <c r="F7" t="s">
+        <v>221</v>
+      </c>
+      <c r="G7" t="s">
+        <v>195</v>
+      </c>
+      <c r="H7" t="s">
+        <v>196</v>
+      </c>
+      <c r="I7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" t="s">
+        <v>222</v>
+      </c>
+      <c r="E8" t="s">
+        <v>223</v>
+      </c>
+      <c r="F8" t="s">
+        <v>224</v>
+      </c>
+      <c r="G8" t="s">
+        <v>198</v>
+      </c>
+      <c r="H8" t="s">
+        <v>199</v>
+      </c>
+      <c r="I8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE6610B7-8CB1-BB4F-B087-1EB669BFFD36}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView zoomScale="183" zoomScaleNormal="183" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" t="s">
+        <v>156</v>
+      </c>
+      <c r="H1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H2" t="s">
+        <v>160</v>
+      </c>
+      <c r="I2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G3" t="s">
+        <v>162</v>
+      </c>
+      <c r="H3" t="s">
+        <v>163</v>
+      </c>
+      <c r="I3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G4" t="s">
+        <v>165</v>
+      </c>
+      <c r="H4" t="s">
+        <v>166</v>
+      </c>
+      <c r="I4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F5" t="s">
+        <v>149</v>
+      </c>
+      <c r="G5" t="s">
+        <v>168</v>
+      </c>
+      <c r="H5" t="s">
+        <v>169</v>
+      </c>
+      <c r="I5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" t="s">
+        <v>150</v>
+      </c>
+      <c r="E6" t="s">
+        <v>151</v>
+      </c>
+      <c r="F6" t="s">
+        <v>152</v>
+      </c>
+      <c r="G6" t="s">
+        <v>171</v>
+      </c>
+      <c r="H6" t="s">
+        <v>172</v>
+      </c>
+      <c r="I6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E7" t="s">
+        <v>154</v>
+      </c>
+      <c r="F7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G7" t="s">
+        <v>174</v>
+      </c>
+      <c r="H7" t="s">
+        <v>175</v>
+      </c>
+      <c r="I7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
double induction exp. data and analysis
</commit_message>
<xml_diff>
--- a/data/malathion-reporter-plate-reader/plate_layouts.xlsx
+++ b/data/malathion-reporter-plate-reader/plate_layouts.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aqib/Desktop/BCCL/koopman-sensor-placement/NC_submission/transcriptome-dynamics-dmd-observability/data/malathion-reporter-plate-reader/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEFD971-40DA-464A-A40B-40606F764358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36289145-2AC6-2148-8AC6-4467B962A7AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{86E41D9F-BC50-BD4C-BFC8-A140258F459E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="4" xr2:uid="{86E41D9F-BC50-BD4C-BFC8-A140258F459E}"/>
   </bookViews>
   <sheets>
     <sheet name="h1_specificity_09.09.22" sheetId="4" r:id="rId1"/>
     <sheet name="neo2_specificity_09.09.22" sheetId="3" r:id="rId2"/>
     <sheet name="h1_specificity_09.13.22" sheetId="1" r:id="rId3"/>
     <sheet name="neo2_specificity_09.13.22" sheetId="2" r:id="rId4"/>
+    <sheet name="h1_specificity_09.28.22" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="243">
   <si>
     <t>6124_control_0</t>
   </si>
@@ -712,6 +713,60 @@
   </si>
   <si>
     <t>4150_fructose_2</t>
+  </si>
+  <si>
+    <t>4736_mal_0</t>
+  </si>
+  <si>
+    <t>4736_mal_1</t>
+  </si>
+  <si>
+    <t>4736_mal_2</t>
+  </si>
+  <si>
+    <t>4736_mal+perm_0</t>
+  </si>
+  <si>
+    <t>4736_mal+perm_1</t>
+  </si>
+  <si>
+    <t>4736_mal+perm_2</t>
+  </si>
+  <si>
+    <t>4736_mal+zeta_0</t>
+  </si>
+  <si>
+    <t>4736_mal+zeta_1</t>
+  </si>
+  <si>
+    <t>4736_mal+zeta_2</t>
+  </si>
+  <si>
+    <t>0953_mal_0</t>
+  </si>
+  <si>
+    <t>0953_mal_1</t>
+  </si>
+  <si>
+    <t>0953_mal_2</t>
+  </si>
+  <si>
+    <t>0953_mal+perm_0</t>
+  </si>
+  <si>
+    <t>0953_mal+perm_1</t>
+  </si>
+  <si>
+    <t>0953_mal+perm_2</t>
+  </si>
+  <si>
+    <t>0953_mal+zeta_0</t>
+  </si>
+  <si>
+    <t>0953_mal+zeta_1</t>
+  </si>
+  <si>
+    <t>0953_mal+zeta_2</t>
   </si>
 </sst>
 </file>
@@ -1323,8 +1378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{012CA423-6E37-EB41-BE63-F2F07D4939DA}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="183" zoomScaleNormal="183" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView zoomScale="183" zoomScaleNormal="183" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1799,9 +1854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE6610B7-8CB1-BB4F-B087-1EB669BFFD36}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView zoomScale="183" zoomScaleNormal="183" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
-    </sheetView>
+    <sheetView zoomScale="183" zoomScaleNormal="183" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2016,4 +2069,136 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFEBC597-DD27-D944-B02F-D80B9B484B5A}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G1" t="s">
+        <v>231</v>
+      </c>
+      <c r="H1" t="s">
+        <v>232</v>
+      </c>
+      <c r="I1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" t="s">
+        <v>237</v>
+      </c>
+      <c r="E3" t="s">
+        <v>238</v>
+      </c>
+      <c r="F3" t="s">
+        <v>239</v>
+      </c>
+      <c r="G3" t="s">
+        <v>240</v>
+      </c>
+      <c r="H3" t="s">
+        <v>241</v>
+      </c>
+      <c r="I3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>